<commit_message>
Aula 5 - 3 para natal dia anrterior
</commit_message>
<xml_diff>
--- a/Aula5/DRE.xlsx
+++ b/Aula5/DRE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Empreendedor\Aulas Excel Basico\Smart-Planning\Aula5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u100054\Desktop\aprendizado\Aulas Excel Basico\Fenrir\Aula5\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="DRE" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -508,10 +508,10 @@
   <dimension ref="B3:V15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>